<commit_message>
Reflections, Planes, and fixed Compute Device.
</commit_message>
<xml_diff>
--- a/work.xlsx
+++ b/work.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan Breit\AppData\Roaming\Emacs\Western\10\Science\Raytracer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98277D59-BC05-4C42-81E7-5C5C00C15040}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802A5E50-C51D-4F1E-BA6B-F7B841EA5F25}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{8BDDFE12-824E-45FA-83D3-7A8815718D2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -140,12 +140,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="46" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
@@ -477,28 +477,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -506,29 +506,29 @@
       <c r="A3" s="1">
         <v>43407</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>0.77083333333333337</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D14" si="0">C3-B3</f>
         <v>0.22916666666666674</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="6">
         <f>SUM(D3:D100)</f>
-        <v>0.85069444444444453</v>
+        <v>1.1277777777777778</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43408</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>0.78125</v>
       </c>
       <c r="D4" s="2">
@@ -540,10 +540,10 @@
       <c r="A5" s="1">
         <v>43413</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>0.3611111111111111</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>0.55555555555555558</v>
       </c>
       <c r="D5" s="2">
@@ -555,10 +555,10 @@
       <c r="A6" s="1">
         <v>43414</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>0.52083333333333337</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>0.75</v>
       </c>
       <c r="D6" s="2">
@@ -567,112 +567,119 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="A7" s="1">
+        <v>43428</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.81874999999999998</v>
+      </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.27708333333333335</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Materials Done. Scenes and Meshes started.
</commit_message>
<xml_diff>
--- a/work.xlsx
+++ b/work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan Breit\AppData\Roaming\Emacs\Western\10\Science\Raytracer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802A5E50-C51D-4F1E-BA6B-F7B841EA5F25}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0DBDE0-13AB-4600-9EFD-FB00E3EE6F55}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{8BDDFE12-824E-45FA-83D3-7A8815718D2E}"/>
   </bookViews>
@@ -142,10 +142,10 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="46" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="46" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
@@ -466,7 +466,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,13 +477,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -516,9 +516,9 @@
         <f t="shared" ref="D3:D14" si="0">C3-B3</f>
         <v>0.22916666666666674</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <f>SUM(D3:D100)</f>
-        <v>1.1277777777777778</v>
+        <v>1.7319444444444443</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -582,19 +582,33 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="A8" s="1">
+        <v>43430</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.85416666666666663</v>
+      </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.13194444444444442</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="1">
+        <v>43431</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.88888888888888884</v>
+      </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.47222222222222215</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Git is really annoying
</commit_message>
<xml_diff>
--- a/work.xlsx
+++ b/work.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan Breit\AppData\Roaming\Emacs\Western\10\Science\Raytracer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan Breit\Documents\Raytracer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB034C9-5DFA-45ED-8AAA-BB73183D8B59}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2035A9-1F43-405B-9CB5-32B9067EA2F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{8BDDFE12-824E-45FA-83D3-7A8815718D2E}"/>
+    <workbookView xWindow="2445" yWindow="1545" windowWidth="21600" windowHeight="11775" xr2:uid="{8BDDFE12-824E-45FA-83D3-7A8815718D2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Time</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Before starting this.</t>
+  </si>
+  <si>
+    <t>Beginning Work Again</t>
   </si>
 </sst>
 </file>
@@ -148,17 +151,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -480,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0B2295-7B48-4F47-B6EF-470B7C5476AB}">
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,13 +499,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -518,17 +525,17 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
       <c r="D3" s="2">
         <v>0.83333333333333337</v>
       </c>
       <c r="E3" s="5">
         <f>SUM(D3:D99)</f>
-        <v>7.5083333333333337</v>
+        <v>7.469444444444445</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -752,7 +759,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" ref="D18:D29" si="2">C18-B18</f>
+        <f t="shared" ref="D18:D32" si="2">C18-B18</f>
         <v>0.58333333333333326</v>
       </c>
     </row>
@@ -877,22 +884,67 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
+      <c r="A27" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
       <c r="D27" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>43530</v>
+      </c>
+      <c r="B28" s="6">
+        <v>0.53888888888888886</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="D28" s="2">
         <f t="shared" si="2"/>
+        <v>0.16944444444444451</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>43531</v>
+      </c>
+      <c r="B29" s="6">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="2"/>
+        <v>0.25000000000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>43532</v>
+      </c>
+      <c r="B30" s="6">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="2">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D29" s="2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -901,9 +953,10 @@
       <c r="D1048576" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A27:C27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed build systems, started ui, fixed average func, and implemented k-d tree
</commit_message>
<xml_diff>
--- a/work.xlsx
+++ b/work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan Breit\Documents\Raytracer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4711D179-157B-4282-A9FE-46BDB9F64D6B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F634F6D-7F50-49D6-8E08-BC7EEE02846B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8BDDFE12-824E-45FA-83D3-7A8815718D2E}"/>
   </bookViews>
@@ -487,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0B2295-7B48-4F47-B6EF-470B7C5476AB}">
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
       </c>
       <c r="E3" s="5">
         <f>SUM(D3:D99)</f>
-        <v>8.2611111111111128</v>
+        <v>9.3444444444444468</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -956,14 +956,17 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>43537</v>
+        <v>43538</v>
       </c>
       <c r="B32" s="6">
-        <v>0.5</v>
+        <v>0.41597222222222219</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0.99930555555555556</v>
       </c>
       <c r="D32" s="2">
         <f t="shared" si="2"/>
-        <v>-0.5</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="1048576" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UI update and integrators split
</commit_message>
<xml_diff>
--- a/work.xlsx
+++ b/work.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan Breit\Documents\Raytracer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3BC344-63FF-41A6-AF97-8288CCA15B52}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D88A04D-FB5D-47AC-968F-3986806C27B4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8BDDFE12-824E-45FA-83D3-7A8815718D2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8BDDFE12-824E-45FA-83D3-7A8815718D2E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hours" sheetId="1" r:id="rId1"/>
+    <sheet name="Bugs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Time</t>
   </si>
@@ -49,6 +50,27 @@
   </si>
   <si>
     <t>Beginning Work Again</t>
+  </si>
+  <si>
+    <t>Bugs</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>on going issue: kernel compilation randomly taking a lot of time</t>
+  </si>
+  <si>
+    <t>raytracer.c/parallel.c</t>
+  </si>
+  <si>
+    <t>loader not robust, can crash if scene format not correct</t>
+  </si>
+  <si>
+    <t>loader.c</t>
   </si>
 </sst>
 </file>
@@ -98,7 +120,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -144,6 +166,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="4"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -151,7 +195,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -159,6 +203,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -166,6 +213,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -487,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0B2295-7B48-4F47-B6EF-470B7C5476AB}">
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,13 +558,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -525,11 +584,11 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="2">
         <v>0.83333333333333337</v>
       </c>
@@ -759,7 +818,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" ref="D18:D32" si="2">C18-B18</f>
+        <f t="shared" ref="D18:D31" si="2">C18-B18</f>
         <v>0.58333333333333326</v>
       </c>
     </row>
@@ -884,11 +943,11 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
       <c r="D27" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1120,4 +1179,159 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B735917-E70E-447D-8687-3870E834E8B2}">
+  <dimension ref="A1:E1048576"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14">
+        <v>43549</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14">
+        <v>43549</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="1048575" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1048576" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1048576" s="7"/>
+      <c r="B1048576" s="12"/>
+      <c r="C1048576" s="12"/>
+      <c r="D1048576" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B1048576:D1048576"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final Windows Push Before Presentation.
</commit_message>
<xml_diff>
--- a/work.xlsx
+++ b/work.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan Breit\Documents\Raytracer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D88A04D-FB5D-47AC-968F-3986806C27B4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14B585A-0CBD-4E01-871D-039B8004FFD4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8BDDFE12-824E-45FA-83D3-7A8815718D2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8BDDFE12-824E-45FA-83D3-7A8815718D2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hours" sheetId="1" r:id="rId1"/>
     <sheet name="Bugs" sheetId="2" r:id="rId2"/>
+    <sheet name="Times" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Time</t>
   </si>
@@ -72,15 +73,40 @@
   <si>
     <t>loader.c</t>
   </si>
+  <si>
+    <t>ISSUE: Never ended up using this</t>
+  </si>
+  <si>
+    <t>everywhere</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Cycles GPU</t>
+  </si>
+  <si>
+    <t>Cycles CPU</t>
+  </si>
+  <si>
+    <t>My Path Tracer</t>
+  </si>
+  <si>
+    <t># of samples</t>
+  </si>
+  <si>
+    <t>Buddha</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="mm:ss.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +137,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -120,7 +162,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -188,14 +230,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -204,6 +257,9 @@
     <xf numFmtId="46" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -215,21 +271,29 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="4" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="5" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
     <cellStyle name="Total" xfId="3" builtinId="25"/>
@@ -245,6 +309,2145 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Norway Scene</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>My Path Tracer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Times!$E$3:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$H$3:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.9790509259259261E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9567129629629629E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1870717592592592E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.450439814814815E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-196C-4414-B3E9-A7E1F9C1AA5A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cycles GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Times!$E$3:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$F$3:$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0995370370370371E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1715277777777779E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3108796296296289E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.543518518518518E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-196C-4414-B3E9-A7E1F9C1AA5A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cycles CPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Times!$E$3:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$G$3:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.8329861111111112E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2884259259259256E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0591087962962964E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1364699074074071E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-196C-4414-B3E9-A7E1F9C1AA5A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="85379776"/>
+        <c:axId val="85380104"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="85379776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="85380104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="85380104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="mm:ss.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="85379776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Buddha</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$H$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>My Path Tracer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Times!$E$9:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$H$9:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0208333333333338E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0633101851851849E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.5603009259259254E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6122685185185187E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B537-43A0-BECA-BB4AA96A93A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$F$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cycles GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Times!$E$9:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$F$9:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.8877314814814814E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3773148148148148E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0486111111111111E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.087615740740741E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B537-43A0-BECA-BB4AA96A93A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$G$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cycles CPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Times!$E$9:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$G$9:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5.6932870370370373E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.112962962962963E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2157407407407408E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4026620370370365E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B537-43A0-BECA-BB4AA96A93A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="648871088"/>
+        <c:axId val="648875024"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="648871088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="648875024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="648875024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="mm:ss.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="648871088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266701</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CF478E4-E9AF-4272-9886-1417CC808B94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>280986</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC3C855A-F776-42D4-9E92-E2FFFE939BAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -558,13 +2761,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -584,11 +2787,11 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="2">
         <v>0.83333333333333337</v>
       </c>
@@ -943,11 +3146,11 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
       <c r="D27" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1185,7 +3388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B735917-E70E-447D-8687-3870E834E8B2}">
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+    <sheetView zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1197,29 +3400,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
       <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14">
+      <c r="A3" s="8">
         <v>43549</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -1232,7 +3435,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14">
+      <c r="A4" s="8">
         <v>43549</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -1245,11 +3448,17 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="8">
+        <v>43559</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
@@ -1316,22 +3525,307 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B1048576:D1048576"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B1048576:D1048576"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624F4620-E231-45AE-BE00-1414527F1DEE}">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:11" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="19"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17">
+        <v>256</v>
+      </c>
+      <c r="F3" s="18">
+        <v>1.0995370370370371E-3</v>
+      </c>
+      <c r="G3" s="18">
+        <v>2.8329861111111112E-3</v>
+      </c>
+      <c r="H3" s="18">
+        <v>2.9790509259259261E-4</v>
+      </c>
+      <c r="K3" s="19"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17">
+        <v>512</v>
+      </c>
+      <c r="F4" s="18">
+        <v>2.1715277777777779E-3</v>
+      </c>
+      <c r="G4" s="18">
+        <v>5.2884259259259256E-3</v>
+      </c>
+      <c r="H4" s="18">
+        <v>5.9567129629629629E-4</v>
+      </c>
+      <c r="K4" s="19"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17">
+        <v>1024</v>
+      </c>
+      <c r="F5" s="18">
+        <v>4.3108796296296289E-3</v>
+      </c>
+      <c r="G5" s="18">
+        <v>1.0591087962962964E-2</v>
+      </c>
+      <c r="H5" s="18">
+        <v>1.1870717592592592E-3</v>
+      </c>
+      <c r="K5" s="19"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17">
+        <v>2048</v>
+      </c>
+      <c r="F6" s="18">
+        <v>8.543518518518518E-3</v>
+      </c>
+      <c r="G6" s="18">
+        <v>2.1364699074074071E-2</v>
+      </c>
+      <c r="H6" s="18">
+        <v>2.450439814814815E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="1:11" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17">
+        <v>256</v>
+      </c>
+      <c r="F9" s="18">
+        <v>2.8877314814814814E-4</v>
+      </c>
+      <c r="G9" s="18">
+        <v>5.6932870370370373E-4</v>
+      </c>
+      <c r="H9" s="18">
+        <v>2.0208333333333338E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C10" s="18"/>
+      <c r="E10" s="17">
+        <v>512</v>
+      </c>
+      <c r="F10" s="18">
+        <v>5.3773148148148148E-4</v>
+      </c>
+      <c r="G10" s="18">
+        <v>1.112962962962963E-3</v>
+      </c>
+      <c r="H10" s="18">
+        <v>4.0633101851851849E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C11" s="18"/>
+      <c r="E11" s="17">
+        <v>1024</v>
+      </c>
+      <c r="F11" s="18">
+        <v>1.0486111111111111E-3</v>
+      </c>
+      <c r="G11" s="18">
+        <v>2.2157407407407408E-3</v>
+      </c>
+      <c r="H11" s="18">
+        <v>7.5603009259259254E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="18"/>
+      <c r="E12" s="17">
+        <v>2048</v>
+      </c>
+      <c r="F12" s="18">
+        <v>2.087615740740741E-3</v>
+      </c>
+      <c r="G12" s="18">
+        <v>4.4026620370370365E-3</v>
+      </c>
+      <c r="H12" s="18">
+        <v>1.6122685185185187E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="18"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="18"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C15" s="18"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C16" s="18"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="18"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="18"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="18"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="18"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="18"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="18"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="18"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="18"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="18"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="18"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="18"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="E7:H7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
A bunch of small stuff
</commit_message>
<xml_diff>
--- a/work.xlsx
+++ b/work.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan Breit\Documents\Raytracer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14B585A-0CBD-4E01-871D-039B8004FFD4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53545935-0B86-46A2-86F7-2CB6A4E5F800}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8BDDFE12-824E-45FA-83D3-7A8815718D2E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8BDDFE12-824E-45FA-83D3-7A8815718D2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hours" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Time</t>
   </si>
@@ -97,6 +97,9 @@
   <si>
     <t>Buddha</t>
   </si>
+  <si>
+    <t>Indigo Renderer</t>
+  </si>
 </sst>
 </file>
 
@@ -104,9 +107,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="mm:ss.00"/>
+    <numFmt numFmtId="165" formatCode="mm:ss.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,16 +156,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -239,16 +255,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -262,6 +294,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5" applyFill="1"/>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="8" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="47" fontId="6" fillId="2" borderId="8" xfId="6" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -271,30 +310,26 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
     <cellStyle name="Heading 1" xfId="4" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="5" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="6" builtinId="21"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
     <cellStyle name="Total" xfId="3" builtinId="25"/>
   </cellStyles>
@@ -392,7 +427,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Times!$H$2</c:f>
+              <c:f>Times!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -434,21 +469,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Times!$H$3:$H$6</c:f>
+              <c:f>Times!$I$3:$I$6</c:f>
               <c:numCache>
                 <c:formatCode>mm:ss.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.9790509259259261E-4</c:v>
+                  <c:v>2.2206018518518516E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.9567129629629629E-4</c:v>
+                  <c:v>4.4510416666666673E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1870717592592592E-3</c:v>
+                  <c:v>8.8773148148148153E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.450439814814815E-3</c:v>
+                  <c:v>1.7786689814814816E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -460,8 +495,59 @@
           </c:extLst>
         </c:ser>
         <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Indigo Renderer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$H$3:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.7777777777777778E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.6712962962962956E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1342592592592591E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2106481481481478E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E796-4D46-8902-7B6B7D30A712}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Times!$F$2</c:f>
@@ -533,7 +619,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Times!$G$2</c:f>
@@ -583,7 +669,7 @@
                 <c:formatCode>mm:ss.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.8329861111111112E-3</c:v>
+                  <c:v>2.8356481481481479E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5.2884259259259256E-3</c:v>
@@ -623,6 +709,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t># of Samples</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -688,6 +829,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Render Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="mm:ss.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -834,7 +1030,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-CA"/>
-              <a:t>Buddha</a:t>
+              <a:t>Buddha Scene</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -876,11 +1072,62 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
               <c:f>Times!$H$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Indigo Renderer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$H$9:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.7777777777777778E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5555555555555556E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0995370370370371E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1874999999999998E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9F74-434B-8415-65D22064BA30}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$I$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -922,21 +1169,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Times!$H$9:$H$12</c:f>
+              <c:f>Times!$I$9:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>mm:ss.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.0208333333333338E-4</c:v>
+                  <c:v>4.078587962962963E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0633101851851849E-4</c:v>
+                  <c:v>8.0858796296296288E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.5603009259259254E-4</c:v>
+                  <c:v>1.6228587962962965E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6122685185185187E-3</c:v>
+                  <c:v>3.1877893518518514E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -949,7 +1196,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Times!$F$8</c:f>
@@ -999,16 +1246,16 @@
                 <c:formatCode>mm:ss.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.8877314814814814E-4</c:v>
+                  <c:v>1.1960648148148147E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.3773148148148148E-4</c:v>
+                  <c:v>2.3379629629629631E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0486111111111111E-3</c:v>
+                  <c:v>4.6232638888888886E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.087615740740741E-3</c:v>
+                  <c:v>9.1898148148148139E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1021,7 +1268,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Times!$G$8</c:f>
@@ -1071,16 +1318,16 @@
                 <c:formatCode>mm:ss.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.6932870370370373E-4</c:v>
+                  <c:v>2.7674768518518521E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.112962962962963E-3</c:v>
+                  <c:v>5.5199074074074074E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2157407407407408E-3</c:v>
+                  <c:v>1.1075578703703704E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.4026620370370365E-3</c:v>
+                  <c:v>2.2291087962962964E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1111,6 +1358,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t># of Samples</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1176,6 +1478,1326 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Render Times</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="mm:ss.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="648871088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Norway Scene</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>My Path Tracer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Times!$E$3:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$I$3:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.2206018518518516E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4510416666666673E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.8773148148148153E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7786689814814816E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F6EE-40F5-A1C9-E7F863BAE2EB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cycles GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Times!$E$3:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$F$3:$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0995370370370371E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1715277777777779E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3108796296296289E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.543518518518518E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F6EE-40F5-A1C9-E7F863BAE2EB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cycles CPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Times!$E$3:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$G$3:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.8356481481481479E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2884259259259256E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0591087962962964E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1364699074074071E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F6EE-40F5-A1C9-E7F863BAE2EB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="85379776"/>
+        <c:axId val="85380104"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Times!$H$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Indigo Renderer</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Times!$H$3:$H$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>mm:ss.00</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>2.7777777777777778E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>5.6712962962962956E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.1342592592592591E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2.2106481481481478E-3</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-F6EE-40F5-A1C9-E7F863BAE2EB}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="85379776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t># of Samples</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="85380104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="85380104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Render Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="mm:ss.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="85379776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Buddha Scene</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$I$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>My Path Tracer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Times!$E$9:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$I$9:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.078587962962963E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0858796296296288E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6228587962962965E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1877893518518514E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5539-419C-9847-454608C42B0D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$F$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cycles GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Times!$E$9:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$F$9:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.1960648148148147E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3379629629629631E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.6232638888888886E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.1898148148148139E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5539-419C-9847-454608C42B0D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$G$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cycles CPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Times!$E$9:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$G$9:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.7674768518518521E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5199074074074074E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1075578703703704E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2291087962962964E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5539-419C-9847-454608C42B0D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="648871088"/>
+        <c:axId val="648875024"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="648871088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t># of Samples</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="648875024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="648875024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Render Times</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="mm:ss.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1367,6 +2989,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1871,6 +3573,1012 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2414,13 +5122,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>280986</xdr:colOff>
+      <xdr:colOff>280985</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
@@ -2442,6 +5150,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C66B15CD-BF3F-4707-A33D-2F8624338887}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>147639</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>166689</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D03121D6-74CA-4FC7-A586-6947A3683B64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2761,13 +5545,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -2787,11 +5571,11 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
       <c r="D3" s="2">
         <v>0.83333333333333337</v>
       </c>
@@ -3146,11 +5930,11 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
       <c r="D27" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3400,23 +6184,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
       <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
@@ -3425,11 +6209,11 @@
       <c r="A3" s="8">
         <v>43549</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21"/>
       <c r="E3" s="7" t="s">
         <v>12</v>
       </c>
@@ -3438,11 +6222,11 @@
       <c r="A4" s="8">
         <v>43549</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
       <c r="E4" s="7" t="s">
         <v>14</v>
       </c>
@@ -3451,77 +6235,77 @@
       <c r="A5" s="8">
         <v>43559</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
       <c r="E5" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="13"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
       <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="13"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
       <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
       <c r="E13" s="7"/>
     </row>
     <row r="1048575" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="1048576" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1048576" s="7"/>
-      <c r="B1048576" s="12"/>
-      <c r="C1048576" s="12"/>
-      <c r="D1048576" s="13"/>
+      <c r="B1048576" s="20"/>
+      <c r="C1048576" s="20"/>
+      <c r="D1048576" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3549,8 +6333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624F4620-E231-45AE-BE00-1414527F1DEE}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="Y16" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3563,260 +6347,291 @@
     <col min="6" max="6" width="19.5703125" customWidth="1"/>
     <col min="7" max="7" width="24.28515625" customWidth="1"/>
     <col min="8" max="8" width="21.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="15" t="s">
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:11" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="20" t="s">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="19"/>
+      <c r="K2" s="12"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10">
         <v>256</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="14">
         <v>1.0995370370370371E-3</v>
       </c>
-      <c r="G3" s="18">
-        <v>2.8329861111111112E-3</v>
-      </c>
-      <c r="H3" s="18">
-        <v>2.9790509259259261E-4</v>
-      </c>
-      <c r="K3" s="19"/>
+      <c r="G3" s="14">
+        <v>2.8356481481481479E-3</v>
+      </c>
+      <c r="H3" s="14">
+        <v>2.7777777777777778E-4</v>
+      </c>
+      <c r="I3" s="14">
+        <v>2.2206018518518516E-4</v>
+      </c>
+      <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10">
         <v>512</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="14">
         <v>2.1715277777777779E-3</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="14">
         <v>5.2884259259259256E-3</v>
       </c>
-      <c r="H4" s="18">
-        <v>5.9567129629629629E-4</v>
-      </c>
-      <c r="K4" s="19"/>
+      <c r="H4" s="14">
+        <v>5.6712962962962956E-4</v>
+      </c>
+      <c r="I4" s="14">
+        <v>4.4510416666666673E-4</v>
+      </c>
+      <c r="K4" s="12"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10">
         <v>1024</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="14">
         <v>4.3108796296296289E-3</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="14">
         <v>1.0591087962962964E-2</v>
       </c>
-      <c r="H5" s="18">
-        <v>1.1870717592592592E-3</v>
-      </c>
-      <c r="K5" s="19"/>
+      <c r="H5" s="14">
+        <v>1.1342592592592591E-3</v>
+      </c>
+      <c r="I5" s="14">
+        <v>8.8773148148148153E-4</v>
+      </c>
+      <c r="K5" s="12"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10">
         <v>2048</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="14">
         <v>8.543518518518518E-3</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="14">
         <v>2.1364699074074071E-2</v>
       </c>
-      <c r="H6" s="18">
-        <v>2.450439814814815E-3</v>
+      <c r="H6" s="14">
+        <v>2.2106481481481478E-3</v>
+      </c>
+      <c r="I6" s="14">
+        <v>1.7786689814814816E-3</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="15" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:11" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="20" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10">
         <v>256</v>
       </c>
-      <c r="F9" s="18">
-        <v>2.8877314814814814E-4</v>
-      </c>
-      <c r="G9" s="18">
-        <v>5.6932870370370373E-4</v>
-      </c>
-      <c r="H9" s="18">
-        <v>2.0208333333333338E-4</v>
+      <c r="F9" s="14">
+        <v>1.1960648148148147E-3</v>
+      </c>
+      <c r="G9" s="14">
+        <v>2.7674768518518521E-3</v>
+      </c>
+      <c r="H9" s="15">
+        <v>2.7777777777777778E-4</v>
+      </c>
+      <c r="I9" s="14">
+        <v>4.078587962962963E-4</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C10" s="18"/>
-      <c r="E10" s="17">
+      <c r="C10" s="11"/>
+      <c r="E10" s="10">
         <v>512</v>
       </c>
-      <c r="F10" s="18">
-        <v>5.3773148148148148E-4</v>
-      </c>
-      <c r="G10" s="18">
-        <v>1.112962962962963E-3</v>
-      </c>
-      <c r="H10" s="18">
-        <v>4.0633101851851849E-4</v>
+      <c r="F10" s="14">
+        <v>2.3379629629629631E-3</v>
+      </c>
+      <c r="G10" s="14">
+        <v>5.5199074074074074E-3</v>
+      </c>
+      <c r="H10" s="15">
+        <v>5.5555555555555556E-4</v>
+      </c>
+      <c r="I10" s="14">
+        <v>8.0858796296296288E-4</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C11" s="18"/>
-      <c r="E11" s="17">
+      <c r="C11" s="11"/>
+      <c r="E11" s="10">
         <v>1024</v>
       </c>
-      <c r="F11" s="18">
-        <v>1.0486111111111111E-3</v>
-      </c>
-      <c r="G11" s="18">
-        <v>2.2157407407407408E-3</v>
-      </c>
-      <c r="H11" s="18">
-        <v>7.5603009259259254E-4</v>
+      <c r="F11" s="14">
+        <v>4.6232638888888886E-3</v>
+      </c>
+      <c r="G11" s="14">
+        <v>1.1075578703703704E-2</v>
+      </c>
+      <c r="H11" s="15">
+        <v>1.0995370370370371E-3</v>
+      </c>
+      <c r="I11" s="14">
+        <v>1.6228587962962965E-3</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C12" s="18"/>
-      <c r="E12" s="17">
+      <c r="C12" s="11"/>
+      <c r="E12" s="10">
         <v>2048</v>
       </c>
-      <c r="F12" s="18">
-        <v>2.087615740740741E-3</v>
-      </c>
-      <c r="G12" s="18">
-        <v>4.4026620370370365E-3</v>
-      </c>
-      <c r="H12" s="18">
-        <v>1.6122685185185187E-3</v>
+      <c r="F12" s="14">
+        <v>9.1898148148148139E-3</v>
+      </c>
+      <c r="G12" s="14">
+        <v>2.2291087962962964E-2</v>
+      </c>
+      <c r="H12" s="15">
+        <v>2.1874999999999998E-3</v>
+      </c>
+      <c r="I12" s="14">
+        <v>3.1877893518518514E-3</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C13" s="18"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
+      <c r="C13" s="11"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="18"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
+      <c r="C14" s="11"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C15" s="18"/>
+      <c r="C15" s="11"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C16" s="18"/>
+      <c r="C16" s="11"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="18"/>
+      <c r="C17" s="11"/>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="18"/>
+      <c r="C18" s="11"/>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="18"/>
+      <c r="C19" s="11"/>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="18"/>
+      <c r="C20" s="11"/>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="18"/>
+      <c r="C21" s="11"/>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="18"/>
+      <c r="C22" s="11"/>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="18"/>
+      <c r="C23" s="11"/>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" s="18"/>
+      <c r="C24" s="11"/>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="18"/>
+      <c r="C25" s="11"/>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" s="18"/>
+      <c r="C26" s="11"/>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C27" s="18"/>
+      <c r="C27" s="11"/>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C28" s="18"/>
+      <c r="C28" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>